<commit_message>
Add option for parse main key column
</commit_message>
<xml_diff>
--- a/Examples/test_data/BasicDemoData.xlsx
+++ b/Examples/test_data/BasicDemoData.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\atthaboon\Documents\SourceCode\Github\CoreRPAHive\Examples\test_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21BF8AD-0EA7-4900-BEAB-E437DBFE4805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4954104D-855B-48FE-8DB1-F1EBF0F61B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CF74247-3540-4F9E-A6D4-E7EEBD1CE39F}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="29070" windowHeight="16500" xr2:uid="{3CF74247-3540-4F9E-A6D4-E7EEBD1CE39F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -473,7 +469,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Clean up example script
</commit_message>
<xml_diff>
--- a/Examples/test_data/BasicDemoData.xlsx
+++ b/Examples/test_data/BasicDemoData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4954104D-855B-48FE-8DB1-F1EBF0F61B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{12EB1EC5-3603-45C7-93D3-81C744DF294B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="29070" windowHeight="16500" xr2:uid="{3CF74247-3540-4F9E-A6D4-E7EEBD1CE39F}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="29100" windowHeight="16500" xr2:uid="{3CF74247-3540-4F9E-A6D4-E7EEBD1CE39F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -469,7 +463,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add support under score replace the new line
</commit_message>
<xml_diff>
--- a/Examples/test_data/BasicDemoData.xlsx
+++ b/Examples/test_data/BasicDemoData.xlsx
@@ -1,62 +1,118 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\atthaboon\Documents\GitHub\robotframework-ExcelDataDriver\Examples\test_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376AE121-FB99-4C42-874E-8C698E9425DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2685" yWindow="2685" windowWidth="29100" windowHeight="16500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="3060" yWindow="1710" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+  <si>
+    <t>[Status]</t>
+  </si>
+  <si>
+    <t>[Log Message]</t>
+  </si>
+  <si>
+    <t>[Screenshot]</t>
+  </si>
+  <si>
+    <t>[Tags]</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>demo1</t>
+  </si>
+  <si>
+    <t>Welcome1</t>
+  </si>
+  <si>
+    <t>demo@demo.com</t>
+  </si>
+  <si>
+    <t>demo2</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>demo3</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>Data
+New line</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999816888943144"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -89,18 +145,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,147 +468,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="15.5703125" customWidth="1" min="2" max="2"/>
-    <col width="14.28515625" customWidth="1" min="3" max="3"/>
-    <col width="8.140625" customWidth="1" min="4" max="4"/>
-    <col width="14.5703125" customWidth="1" min="5" max="5"/>
-    <col width="14.140625" customWidth="1" min="6" max="6"/>
-    <col width="17.7109375" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>[Status2]</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>[Log Message2]</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>[Screenshot2]</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>[Tags2]</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>[Status]</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>[Log Message]</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>[Screenshot]</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>[Tags]</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2">
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>demo1</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>Welcome1</t>
-        </is>
-      </c>
-      <c r="K2" s="4" t="inlineStr">
-        <is>
-          <t>demo@demo.com</t>
-        </is>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="E3" s="2" t="n"/>
-      <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>demo2</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>Welcome1</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>demo</t>
-        </is>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="2" t="n"/>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="2" t="inlineStr">
-        <is>
-          <t>demo3</t>
-        </is>
-      </c>
-      <c r="J4" s="2" t="n"/>
-      <c r="K4" s="4" t="inlineStr">
-        <is>
-          <t>demo@demo.com</t>
-        </is>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G4" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" display="mailto:demo@demo.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" display="mailto:demo@demo.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>